<commit_message>
fix prep new data format
</commit_message>
<xml_diff>
--- a/codes/demo_order.xlsx
+++ b/codes/demo_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\pg-dt-portal-for-nz\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\git\DT-PG-NZ\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8507C73C-F80B-445E-9D64-0E9D2FABC2A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA9862C-2E5A-425C-83AF-B62B25D7DC8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7C5B2639-0D78-4248-A766-610DD7AB3DE6}"/>
   </bookViews>
@@ -102,18 +102,6 @@
     <t>Lifestages</t>
   </si>
   <si>
-    <t>Young singles/couples without</t>
-  </si>
-  <si>
-    <t>Mature singles/couples without</t>
-  </si>
-  <si>
-    <t>Senior singles/couples without</t>
-  </si>
-  <si>
-    <t>Retired singles/couples withou</t>
-  </si>
-  <si>
     <t>Family with children &lt;18</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t>Family with children 4-5 years</t>
   </si>
   <si>
-    <t>Family with children 6-12 year</t>
-  </si>
-  <si>
-    <t>Family with children 13-18 yea</t>
-  </si>
-  <si>
     <t>Geographical Area</t>
   </si>
   <si>
@@ -412,6 +394,24 @@
   </si>
   <si>
     <t>socdem_gr</t>
+  </si>
+  <si>
+    <t>young singles/couples without children (&lt;35 years)</t>
+  </si>
+  <si>
+    <t>mature singles/couples without children (35-49 years)</t>
+  </si>
+  <si>
+    <t>senior singles/couples without children (50-64 years)</t>
+  </si>
+  <si>
+    <t>retired singles/couples without children (&gt;65 years)</t>
+  </si>
+  <si>
+    <t>Family with children 6-12 years</t>
+  </si>
+  <si>
+    <t>Family with children 13-18 years</t>
   </si>
 </sst>
 </file>
@@ -1248,15 +1248,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C388E755-3FE2-45B0-A3F4-E1B5FA8EE619}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1264,19 +1264,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1290,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -1350,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -1370,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -1390,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -1410,7 +1410,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -1430,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -1470,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -1490,7 +1490,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -1510,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -1530,7 +1530,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1550,7 +1550,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1570,7 +1570,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -1579,7 +1579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>264343</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1599,7 +1599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>264342</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -1619,7 +1619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>264322</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -1639,7 +1639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>257594</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -1659,7 +1659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>264323</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -1679,7 +1679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>264324</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
@@ -1699,7 +1699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>264325</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -1719,7 +1719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>249920</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
@@ -1739,7 +1739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>305885</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1">
         <v>2</v>
@@ -1759,7 +1759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>264336</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1">
         <v>2</v>
@@ -1779,7 +1779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>264337</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1799,7 +1799,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>264338</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1819,18 +1819,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>243513</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>25</v>
+      <c r="B29" t="s">
+        <v>123</v>
       </c>
       <c r="C29" s="34">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
@@ -1838,19 +1838,20 @@
       <c r="F29" s="33">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>261635</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
+      <c r="B30" t="s">
+        <v>124</v>
       </c>
       <c r="C30" s="35">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E30" s="1">
         <v>2</v>
@@ -1858,19 +1859,20 @@
       <c r="F30" s="33">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>261636</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>27</v>
+      <c r="B31" t="s">
+        <v>125</v>
       </c>
       <c r="C31" s="36">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -1878,19 +1880,20 @@
       <c r="F31" s="33">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>261637</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
+      <c r="B32" t="s">
+        <v>126</v>
       </c>
       <c r="C32" s="37">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1">
         <v>2</v>
@@ -1898,19 +1901,20 @@
       <c r="F32" s="33">
         <v>27</v>
       </c>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>261638</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C33" s="33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -1924,13 +1928,13 @@
         <v>264332</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C34" s="38">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1">
         <v>3</v>
@@ -1944,13 +1948,13 @@
         <v>243519</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C35" s="39">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1">
         <v>4</v>
@@ -1964,13 +1968,13 @@
         <v>264333</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C36" s="40">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -1984,13 +1988,13 @@
         <v>305884</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="C37" s="41">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1">
         <v>3</v>
@@ -2004,13 +2008,13 @@
         <v>255533</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="C38" s="42">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -2024,13 +2028,13 @@
         <v>273503</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C39" s="43">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -2044,13 +2048,13 @@
         <v>264340</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C40" s="45">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1">
         <v>2</v>
@@ -2064,13 +2068,13 @@
         <v>264326</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C41" s="46">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -2084,13 +2088,13 @@
         <v>264329</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C42" s="47">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E42" s="1">
         <v>2</v>
@@ -2104,13 +2108,13 @@
         <v>264328</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C43" s="48">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E43" s="1">
         <v>2</v>
@@ -2124,13 +2128,13 @@
         <v>264327</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C44" s="44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
@@ -2144,13 +2148,13 @@
         <v>264339</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C45" s="49">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E45" s="1">
         <v>2</v>
@@ -2164,13 +2168,13 @@
         <v>800001</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C46" s="50">
         <v>45</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -2184,13 +2188,13 @@
         <v>800002</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C47" s="52">
         <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E47" s="1">
         <v>2</v>
@@ -2204,13 +2208,13 @@
         <v>800003</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C48" s="53">
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E48" s="1">
         <v>2</v>
@@ -2224,13 +2228,13 @@
         <v>800004</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C49" s="54">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E49" s="1">
         <v>2</v>
@@ -2244,13 +2248,13 @@
         <v>800005</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C50" s="55">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E50" s="1">
         <v>2</v>
@@ -2264,13 +2268,13 @@
         <v>800011</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C51" s="51">
         <v>50</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -2284,13 +2288,13 @@
         <v>800012</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C52" s="57">
         <v>51</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -2304,13 +2308,13 @@
         <v>800013</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C53" s="58">
         <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -2324,13 +2328,13 @@
         <v>800014</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C54" s="59">
         <v>53</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E54" s="1">
         <v>2</v>
@@ -2344,13 +2348,13 @@
         <v>284329</v>
       </c>
       <c r="B55" s="61" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C55" s="62">
         <v>54</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -2364,13 +2368,13 @@
         <v>282145</v>
       </c>
       <c r="B56" s="61" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C56" s="56">
         <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E56" s="1">
         <v>2</v>
@@ -2384,13 +2388,13 @@
         <v>284678</v>
       </c>
       <c r="B57" s="61" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C57" s="64">
         <v>56</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E57" s="1">
         <v>2</v>
@@ -2404,13 +2408,13 @@
         <v>287683</v>
       </c>
       <c r="B58" s="61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C58" s="65">
         <v>57</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E58" s="1">
         <v>2</v>
@@ -2424,13 +2428,13 @@
         <v>295537</v>
       </c>
       <c r="B59" s="61" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C59" s="66">
         <v>58</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -2444,13 +2448,13 @@
         <v>296132</v>
       </c>
       <c r="B60" s="61" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C60" s="63">
         <v>59</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E60" s="1">
         <v>2</v>
@@ -2464,13 +2468,13 @@
         <v>299087</v>
       </c>
       <c r="B61" s="61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C61" s="68">
         <v>60</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E61" s="1">
         <v>2</v>
@@ -2484,13 +2488,13 @@
         <v>290954</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C62" s="69">
         <v>61</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -2504,13 +2508,13 @@
         <v>297140</v>
       </c>
       <c r="B63" s="61" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C63" s="70">
         <v>62</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E63" s="1">
         <v>2</v>
@@ -2524,13 +2528,13 @@
         <v>296259</v>
       </c>
       <c r="B64" s="61" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C64" s="67">
         <v>63</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E64" s="1">
         <v>2</v>
@@ -2538,6 +2542,24 @@
       <c r="F64" s="67">
         <v>58</v>
       </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="61"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="61"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="61"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="61"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="61"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>